<commit_message>
Fixed x-axis error in figure S1b and some minor grammatical stuff.
</commit_message>
<xml_diff>
--- a/raw_data/metadata.xlsx
+++ b/raw_data/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/SNOLH_Genomics/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA909115-CB89-114F-8716-519616304CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E33A19C-778E-154D-942A-6B3314F535BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="15980" xr2:uid="{A65F9020-AEF3-134F-925A-DBC4100CC07D}"/>
   </bookViews>
@@ -5065,7 +5065,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3871" uniqueCount="1199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3850" uniqueCount="1197">
   <si>
     <t>SKIA-08</t>
   </si>
@@ -8596,12 +8596,6 @@
   </si>
   <si>
     <t>G1018-03-OSU_CHA-040</t>
-  </si>
-  <si>
-    <t>SHB_-_REMOVE</t>
-  </si>
-  <si>
-    <t>SHB - REMOVE</t>
   </si>
   <si>
     <t>Shoal</t>
@@ -9110,7 +9104,7 @@
   <dimension ref="A1:M488"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E465" sqref="E465:E488"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9129,48 +9123,48 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1188</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1187</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>1183</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>1182</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1194</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1193</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1192</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1191</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1190</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1189</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1188</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1187</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>1186</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>1185</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>1184</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -9178,36 +9172,22 @@
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1178</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>1179</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>1178</v>
-      </c>
-      <c r="G2" s="2" t="s">
         <v>1177</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>1178</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>1178</v>
-      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
-        <v>1177</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>1177</v>
-      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -9215,32 +9195,18 @@
       <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1178</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>1179</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>1178</v>
-      </c>
-      <c r="G3" s="2" t="s">
         <v>1177</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>1178</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>1178</v>
-      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
-        <v>1177</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>1177</v>
-      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -9252,32 +9218,18 @@
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>1178</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>1179</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>1178</v>
-      </c>
-      <c r="G4" s="2" t="s">
         <v>1177</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>1178</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>1178</v>
-      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
-        <v>1177</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>1177</v>
-      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -9621,7 +9573,7 @@
         <v>23</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>1025</v>
@@ -9662,7 +9614,7 @@
         <v>23</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>1025</v>
@@ -9703,7 +9655,7 @@
         <v>23</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>1025</v>
@@ -9744,7 +9696,7 @@
         <v>23</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>1025</v>
@@ -9785,7 +9737,7 @@
         <v>19</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>1025</v>
@@ -9826,7 +9778,7 @@
         <v>22</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>1025</v>
@@ -9867,7 +9819,7 @@
         <v>22</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>1025</v>
@@ -9908,7 +9860,7 @@
         <v>22</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>1025</v>
@@ -9949,7 +9901,7 @@
         <v>24</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>1025</v>
@@ -9990,7 +9942,7 @@
         <v>24</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>1025</v>
@@ -10031,7 +9983,7 @@
         <v>18</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>1025</v>
@@ -10072,7 +10024,7 @@
         <v>18</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>1025</v>
@@ -10113,7 +10065,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>1025</v>
@@ -10154,7 +10106,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>1025</v>
@@ -10195,7 +10147,7 @@
         <v>17</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>1025</v>
@@ -10236,7 +10188,7 @@
         <v>17</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>1025</v>
@@ -10277,7 +10229,7 @@
         <v>17</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>1025</v>
@@ -10318,7 +10270,7 @@
         <v>17</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>1025</v>
@@ -10359,7 +10311,7 @@
         <v>17</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>1025</v>
@@ -10400,7 +10352,7 @@
         <v>17</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>1025</v>
@@ -10441,7 +10393,7 @@
         <v>45</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>1025</v>
@@ -10482,7 +10434,7 @@
         <v>45</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>1025</v>
@@ -10523,7 +10475,7 @@
         <v>45</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>1025</v>
@@ -10564,7 +10516,7 @@
         <v>46</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>1025</v>
@@ -10605,7 +10557,7 @@
         <v>46</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>1025</v>
@@ -10646,7 +10598,7 @@
         <v>46</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>1025</v>
@@ -10687,7 +10639,7 @@
         <v>46</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>1025</v>
@@ -10728,7 +10680,7 @@
         <v>47</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>1025</v>
@@ -10769,7 +10721,7 @@
         <v>47</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>1025</v>
@@ -10810,7 +10762,7 @@
         <v>47</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>1025</v>
@@ -10851,7 +10803,7 @@
         <v>52</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>1025</v>
@@ -10892,7 +10844,7 @@
         <v>52</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>1025</v>
@@ -10933,7 +10885,7 @@
         <v>52</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>1025</v>
@@ -10974,7 +10926,7 @@
         <v>52</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>1025</v>
@@ -11015,7 +10967,7 @@
         <v>55</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>1025</v>
@@ -11056,7 +11008,7 @@
         <v>55</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>1025</v>
@@ -11097,7 +11049,7 @@
         <v>55</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>1025</v>
@@ -11138,7 +11090,7 @@
         <v>55</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>1025</v>
@@ -11179,7 +11131,7 @@
         <v>55</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>1025</v>
@@ -11220,7 +11172,7 @@
         <v>55</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>1025</v>
@@ -11261,7 +11213,7 @@
         <v>85</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>1025</v>
@@ -11300,7 +11252,7 @@
         <v>85</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>1025</v>
@@ -11339,7 +11291,7 @@
         <v>85</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>1025</v>
@@ -11378,7 +11330,7 @@
         <v>73</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>1025</v>
@@ -11417,7 +11369,7 @@
         <v>73</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>1025</v>
@@ -11456,7 +11408,7 @@
         <v>73</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>1025</v>
@@ -11495,7 +11447,7 @@
         <v>73</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>1025</v>
@@ -11534,7 +11486,7 @@
         <v>73</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>1025</v>
@@ -11573,7 +11525,7 @@
         <v>73</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>1025</v>
@@ -11612,7 +11564,7 @@
         <v>74</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>1025</v>
@@ -11651,7 +11603,7 @@
         <v>81</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>66</v>
@@ -11690,7 +11642,7 @@
         <v>87</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>66</v>
@@ -11729,7 +11681,7 @@
         <v>72</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>66</v>
@@ -11768,7 +11720,7 @@
         <v>75</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>66</v>
@@ -11807,7 +11759,7 @@
         <v>75</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>66</v>
@@ -11846,7 +11798,7 @@
         <v>75</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>66</v>
@@ -11885,7 +11837,7 @@
         <v>75</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>66</v>
@@ -11924,7 +11876,7 @@
         <v>75</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>66</v>
@@ -11963,7 +11915,7 @@
         <v>75</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F71" s="7" t="s">
         <v>66</v>
@@ -12002,7 +11954,7 @@
         <v>76</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>66</v>
@@ -12041,7 +11993,7 @@
         <v>76</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>66</v>
@@ -12080,7 +12032,7 @@
         <v>76</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F74" s="7" t="s">
         <v>66</v>
@@ -12119,7 +12071,7 @@
         <v>76</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>66</v>
@@ -12158,7 +12110,7 @@
         <v>76</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>66</v>
@@ -12197,7 +12149,7 @@
         <v>77</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>66</v>
@@ -12236,7 +12188,7 @@
         <v>77</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>66</v>
@@ -12275,7 +12227,7 @@
         <v>77</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>66</v>
@@ -12314,7 +12266,7 @@
         <v>77</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F80" s="7" t="s">
         <v>66</v>
@@ -12353,7 +12305,7 @@
         <v>77</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>66</v>
@@ -12392,7 +12344,7 @@
         <v>77</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F82" s="7" t="s">
         <v>66</v>
@@ -12431,7 +12383,7 @@
         <v>77</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F83" s="7" t="s">
         <v>66</v>
@@ -12470,7 +12422,7 @@
         <v>77</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F84" s="7" t="s">
         <v>66</v>
@@ -12509,7 +12461,7 @@
         <v>77</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F85" s="7" t="s">
         <v>66</v>
@@ -12548,7 +12500,7 @@
         <v>77</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F86" s="7" t="s">
         <v>66</v>
@@ -12587,7 +12539,7 @@
         <v>77</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F87" s="7" t="s">
         <v>66</v>
@@ -12626,7 +12578,7 @@
         <v>86</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F88" s="7" t="s">
         <v>66</v>
@@ -12665,7 +12617,7 @@
         <v>86</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F89" s="7" t="s">
         <v>66</v>
@@ -12704,7 +12656,7 @@
         <v>88</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F90" s="7" t="s">
         <v>66</v>
@@ -12743,7 +12695,7 @@
         <v>89</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F91" s="7" t="s">
         <v>66</v>
@@ -12782,7 +12734,7 @@
         <v>78</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F92" s="7" t="s">
         <v>66</v>
@@ -12821,7 +12773,7 @@
         <v>79</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F93" s="7" t="s">
         <v>66</v>
@@ -12860,7 +12812,7 @@
         <v>80</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F94" s="7" t="s">
         <v>66</v>
@@ -12899,7 +12851,7 @@
         <v>80</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F95" s="7" t="s">
         <v>66</v>
@@ -12938,7 +12890,7 @@
         <v>80</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F96" s="7" t="s">
         <v>66</v>
@@ -12977,7 +12929,7 @@
         <v>105</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F97" s="7" t="s">
         <v>66</v>
@@ -13018,7 +12970,7 @@
         <v>105</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F98" s="7" t="s">
         <v>66</v>
@@ -13059,7 +13011,7 @@
         <v>105</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F99" s="7" t="s">
         <v>66</v>
@@ -13100,7 +13052,7 @@
         <v>106</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F100" s="7" t="s">
         <v>66</v>
@@ -13141,7 +13093,7 @@
         <v>106</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F101" s="7" t="s">
         <v>66</v>
@@ -13182,7 +13134,7 @@
         <v>106</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F102" s="7" t="s">
         <v>66</v>
@@ -13223,7 +13175,7 @@
         <v>106</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F103" s="7" t="s">
         <v>66</v>
@@ -13264,7 +13216,7 @@
         <v>106</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F104" s="7" t="s">
         <v>66</v>
@@ -13305,7 +13257,7 @@
         <v>106</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F105" s="7" t="s">
         <v>66</v>
@@ -13346,7 +13298,7 @@
         <v>106</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F106" s="7" t="s">
         <v>66</v>
@@ -13387,7 +13339,7 @@
         <v>106</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F107" s="7" t="s">
         <v>66</v>
@@ -13428,7 +13380,7 @@
         <v>106</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F108" s="7" t="s">
         <v>66</v>
@@ -13469,7 +13421,7 @@
         <v>106</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F109" s="7" t="s">
         <v>66</v>
@@ -13510,7 +13462,7 @@
         <v>99</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F110" s="7" t="s">
         <v>66</v>
@@ -13551,7 +13503,7 @@
         <v>99</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F111" s="7" t="s">
         <v>66</v>
@@ -13592,7 +13544,7 @@
         <v>99</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F112" s="7" t="s">
         <v>66</v>
@@ -13633,7 +13585,7 @@
         <v>99</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F113" s="7" t="s">
         <v>66</v>
@@ -13674,7 +13626,7 @@
         <v>99</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F114" s="7" t="s">
         <v>66</v>
@@ -13715,7 +13667,7 @@
         <v>100</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F115" s="7" t="s">
         <v>66</v>
@@ -13756,7 +13708,7 @@
         <v>100</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F116" s="7" t="s">
         <v>66</v>
@@ -13797,7 +13749,7 @@
         <v>107</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F117" s="7" t="s">
         <v>66</v>
@@ -13838,7 +13790,7 @@
         <v>101</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F118" s="7" t="s">
         <v>66</v>
@@ -13879,7 +13831,7 @@
         <v>101</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F119" s="7" t="s">
         <v>66</v>
@@ -13920,7 +13872,7 @@
         <v>104</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F120" s="7" t="s">
         <v>66</v>
@@ -13961,7 +13913,7 @@
         <v>104</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F121" s="7" t="s">
         <v>66</v>
@@ -14002,7 +13954,7 @@
         <v>104</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F122" s="7" t="s">
         <v>66</v>
@@ -14043,7 +13995,7 @@
         <v>104</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F123" s="7" t="s">
         <v>66</v>
@@ -14084,7 +14036,7 @@
         <v>104</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F124" s="7" t="s">
         <v>66</v>
@@ -14125,7 +14077,7 @@
         <v>97</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F125" s="7" t="s">
         <v>66</v>
@@ -14166,7 +14118,7 @@
         <v>98</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F126" s="7" t="s">
         <v>66</v>
@@ -14207,7 +14159,7 @@
         <v>98</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F127" s="7" t="s">
         <v>66</v>
@@ -14248,7 +14200,7 @@
         <v>62</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F128" s="2" t="s">
         <v>66</v>
@@ -14289,7 +14241,7 @@
         <v>62</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F129" s="2" t="s">
         <v>66</v>
@@ -14330,7 +14282,7 @@
         <v>62</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F130" s="2" t="s">
         <v>66</v>
@@ -14371,7 +14323,7 @@
         <v>62</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F131" s="2" t="s">
         <v>66</v>
@@ -14412,7 +14364,7 @@
         <v>62</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F132" s="2" t="s">
         <v>66</v>
@@ -14453,7 +14405,7 @@
         <v>62</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F133" s="2" t="s">
         <v>66</v>
@@ -14494,7 +14446,7 @@
         <v>61</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F134" s="2" t="s">
         <v>66</v>
@@ -14535,7 +14487,7 @@
         <v>61</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F135" s="2" t="s">
         <v>66</v>
@@ -14576,7 +14528,7 @@
         <v>61</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F136" s="2" t="s">
         <v>66</v>
@@ -14617,7 +14569,7 @@
         <v>61</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F137" s="2" t="s">
         <v>66</v>
@@ -14658,7 +14610,7 @@
         <v>61</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F138" s="2" t="s">
         <v>66</v>
@@ -14699,7 +14651,7 @@
         <v>61</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F139" s="2" t="s">
         <v>66</v>
@@ -14740,7 +14692,7 @@
         <v>61</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F140" s="2" t="s">
         <v>66</v>
@@ -14781,7 +14733,7 @@
         <v>61</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F141" s="2" t="s">
         <v>66</v>
@@ -14822,7 +14774,7 @@
         <v>61</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F142" s="2" t="s">
         <v>66</v>
@@ -14863,7 +14815,7 @@
         <v>61</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F143" s="2" t="s">
         <v>66</v>
@@ -14904,7 +14856,7 @@
         <v>61</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F144" s="2" t="s">
         <v>66</v>
@@ -14945,7 +14897,7 @@
         <v>61</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F145" s="2" t="s">
         <v>66</v>
@@ -14986,7 +14938,7 @@
         <v>61</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F146" s="2" t="s">
         <v>66</v>
@@ -15027,7 +14979,7 @@
         <v>96</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F147" s="7" t="s">
         <v>66</v>
@@ -15068,7 +15020,7 @@
         <v>96</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F148" s="7" t="s">
         <v>66</v>
@@ -15109,7 +15061,7 @@
         <v>96</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F149" s="7" t="s">
         <v>66</v>
@@ -15150,7 +15102,7 @@
         <v>96</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F150" s="7" t="s">
         <v>66</v>
@@ -15191,7 +15143,7 @@
         <v>96</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F151" s="7" t="s">
         <v>66</v>
@@ -15232,7 +15184,7 @@
         <v>96</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F152" s="7" t="s">
         <v>66</v>
@@ -15273,7 +15225,7 @@
         <v>96</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F153" s="7" t="s">
         <v>66</v>
@@ -15314,7 +15266,7 @@
         <v>96</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F154" s="7" t="s">
         <v>66</v>
@@ -15355,7 +15307,7 @@
         <v>96</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F155" s="7" t="s">
         <v>66</v>
@@ -15396,7 +15348,7 @@
         <v>96</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F156" s="7" t="s">
         <v>66</v>
@@ -15437,7 +15389,7 @@
         <v>96</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F157" s="7" t="s">
         <v>66</v>
@@ -15478,7 +15430,7 @@
         <v>96</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F158" s="7" t="s">
         <v>66</v>
@@ -15519,7 +15471,7 @@
         <v>96</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F159" s="7" t="s">
         <v>66</v>
@@ -15560,7 +15512,7 @@
         <v>96</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F160" s="7" t="s">
         <v>66</v>
@@ -15601,7 +15553,7 @@
         <v>96</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F161" s="7" t="s">
         <v>66</v>
@@ -15642,7 +15594,7 @@
         <v>96</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F162" s="7" t="s">
         <v>66</v>
@@ -15683,7 +15635,7 @@
         <v>96</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F163" s="7" t="s">
         <v>66</v>
@@ -15724,7 +15676,7 @@
         <v>96</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F164" s="7" t="s">
         <v>66</v>
@@ -15765,7 +15717,7 @@
         <v>96</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F165" s="7" t="s">
         <v>66</v>
@@ -15806,7 +15758,7 @@
         <v>96</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F166" s="7" t="s">
         <v>66</v>
@@ -15847,7 +15799,7 @@
         <v>96</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F167" s="7" t="s">
         <v>66</v>
@@ -15888,7 +15840,7 @@
         <v>96</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F168" s="7" t="s">
         <v>66</v>
@@ -15929,7 +15881,7 @@
         <v>96</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F169" s="7" t="s">
         <v>66</v>
@@ -15970,7 +15922,7 @@
         <v>96</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F170" s="7" t="s">
         <v>66</v>
@@ -16011,7 +15963,7 @@
         <v>96</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F171" s="7" t="s">
         <v>66</v>
@@ -16052,7 +16004,7 @@
         <v>96</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F172" s="7" t="s">
         <v>66</v>
@@ -16093,7 +16045,7 @@
         <v>96</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F173" s="7" t="s">
         <v>66</v>
@@ -16134,7 +16086,7 @@
         <v>96</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F174" s="7" t="s">
         <v>66</v>
@@ -16175,7 +16127,7 @@
         <v>96</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F175" s="7" t="s">
         <v>66</v>
@@ -16216,7 +16168,7 @@
         <v>60</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F176" s="2" t="s">
         <v>66</v>
@@ -16257,7 +16209,7 @@
         <v>60</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F177" s="2" t="s">
         <v>66</v>
@@ -16298,7 +16250,7 @@
         <v>26</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F178" s="2" t="s">
         <v>66</v>
@@ -16339,7 +16291,7 @@
         <v>26</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F179" s="2" t="s">
         <v>66</v>
@@ -16380,7 +16332,7 @@
         <v>71</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F180" s="2" t="s">
         <v>66</v>
@@ -16421,7 +16373,7 @@
         <v>71</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F181" s="2" t="s">
         <v>66</v>
@@ -16462,7 +16414,7 @@
         <v>71</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F182" s="2" t="s">
         <v>66</v>
@@ -16503,7 +16455,7 @@
         <v>102</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F183" s="7" t="s">
         <v>66</v>
@@ -16544,7 +16496,7 @@
         <v>102</v>
       </c>
       <c r="E184" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F184" s="7" t="s">
         <v>66</v>
@@ -16585,7 +16537,7 @@
         <v>102</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F185" s="7" t="s">
         <v>66</v>
@@ -16626,7 +16578,7 @@
         <v>102</v>
       </c>
       <c r="E186" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F186" s="7" t="s">
         <v>66</v>
@@ -16667,7 +16619,7 @@
         <v>102</v>
       </c>
       <c r="E187" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F187" s="7" t="s">
         <v>66</v>
@@ -16708,7 +16660,7 @@
         <v>102</v>
       </c>
       <c r="E188" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F188" s="7" t="s">
         <v>66</v>
@@ -16749,7 +16701,7 @@
         <v>103</v>
       </c>
       <c r="E189" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F189" s="7" t="s">
         <v>66</v>
@@ -16790,7 +16742,7 @@
         <v>103</v>
       </c>
       <c r="E190" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F190" s="7" t="s">
         <v>66</v>
@@ -16831,7 +16783,7 @@
         <v>103</v>
       </c>
       <c r="E191" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F191" s="7" t="s">
         <v>66</v>
@@ -16872,7 +16824,7 @@
         <v>94</v>
       </c>
       <c r="E192" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F192" s="7" t="s">
         <v>66</v>
@@ -16913,7 +16865,7 @@
         <v>94</v>
       </c>
       <c r="E193" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F193" s="7" t="s">
         <v>66</v>
@@ -16954,7 +16906,7 @@
         <v>94</v>
       </c>
       <c r="E194" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F194" s="7" t="s">
         <v>66</v>
@@ -16995,7 +16947,7 @@
         <v>94</v>
       </c>
       <c r="E195" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F195" s="7" t="s">
         <v>66</v>
@@ -17036,7 +16988,7 @@
         <v>94</v>
       </c>
       <c r="E196" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F196" s="7" t="s">
         <v>66</v>
@@ -17077,7 +17029,7 @@
         <v>94</v>
       </c>
       <c r="E197" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F197" s="7" t="s">
         <v>66</v>
@@ -17118,7 +17070,7 @@
         <v>94</v>
       </c>
       <c r="E198" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F198" s="7" t="s">
         <v>66</v>
@@ -17159,7 +17111,7 @@
         <v>94</v>
       </c>
       <c r="E199" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F199" s="7" t="s">
         <v>66</v>
@@ -17200,7 +17152,7 @@
         <v>94</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F200" s="7" t="s">
         <v>66</v>
@@ -17241,7 +17193,7 @@
         <v>94</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F201" s="7" t="s">
         <v>66</v>
@@ -17282,7 +17234,7 @@
         <v>94</v>
       </c>
       <c r="E202" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F202" s="7" t="s">
         <v>66</v>
@@ -17323,7 +17275,7 @@
         <v>94</v>
       </c>
       <c r="E203" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F203" s="7" t="s">
         <v>66</v>
@@ -17364,7 +17316,7 @@
         <v>94</v>
       </c>
       <c r="E204" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F204" s="7" t="s">
         <v>66</v>
@@ -17405,7 +17357,7 @@
         <v>94</v>
       </c>
       <c r="E205" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F205" s="7" t="s">
         <v>66</v>
@@ -17446,7 +17398,7 @@
         <v>94</v>
       </c>
       <c r="E206" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F206" s="7" t="s">
         <v>66</v>
@@ -17487,7 +17439,7 @@
         <v>94</v>
       </c>
       <c r="E207" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F207" s="7" t="s">
         <v>66</v>
@@ -17528,7 +17480,7 @@
         <v>94</v>
       </c>
       <c r="E208" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F208" s="7" t="s">
         <v>66</v>
@@ -17569,7 +17521,7 @@
         <v>94</v>
       </c>
       <c r="E209" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F209" s="7" t="s">
         <v>66</v>
@@ -17610,7 +17562,7 @@
         <v>94</v>
       </c>
       <c r="E210" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F210" s="7" t="s">
         <v>66</v>
@@ -17651,7 +17603,7 @@
         <v>95</v>
       </c>
       <c r="E211" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F211" s="7" t="s">
         <v>66</v>
@@ -17692,7 +17644,7 @@
         <v>92</v>
       </c>
       <c r="E212" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F212" s="7" t="s">
         <v>66</v>
@@ -17733,7 +17685,7 @@
         <v>93</v>
       </c>
       <c r="E213" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F213" s="7" t="s">
         <v>66</v>
@@ -17774,7 +17726,7 @@
         <v>93</v>
       </c>
       <c r="E214" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F214" s="7" t="s">
         <v>66</v>
@@ -17815,7 +17767,7 @@
         <v>93</v>
       </c>
       <c r="E215" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F215" s="7" t="s">
         <v>66</v>
@@ -17856,7 +17808,7 @@
         <v>93</v>
       </c>
       <c r="E216" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F216" s="7" t="s">
         <v>66</v>
@@ -17897,7 +17849,7 @@
         <v>93</v>
       </c>
       <c r="E217" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F217" s="7" t="s">
         <v>66</v>
@@ -17938,7 +17890,7 @@
         <v>93</v>
       </c>
       <c r="E218" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F218" s="7" t="s">
         <v>66</v>
@@ -17979,7 +17931,7 @@
         <v>70</v>
       </c>
       <c r="E219" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F219" s="2" t="s">
         <v>66</v>
@@ -18020,7 +17972,7 @@
         <v>63</v>
       </c>
       <c r="E220" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F220" s="2" t="s">
         <v>66</v>
@@ -18061,7 +18013,7 @@
         <v>63</v>
       </c>
       <c r="E221" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F221" s="2" t="s">
         <v>66</v>
@@ -18102,7 +18054,7 @@
         <v>63</v>
       </c>
       <c r="E222" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F222" s="2" t="s">
         <v>66</v>
@@ -18143,7 +18095,7 @@
         <v>63</v>
       </c>
       <c r="E223" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F223" s="2" t="s">
         <v>66</v>
@@ -18184,7 +18136,7 @@
         <v>63</v>
       </c>
       <c r="E224" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F224" s="2" t="s">
         <v>66</v>
@@ -18225,7 +18177,7 @@
         <v>63</v>
       </c>
       <c r="E225" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F225" s="2" t="s">
         <v>66</v>
@@ -18266,7 +18218,7 @@
         <v>63</v>
       </c>
       <c r="E226" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F226" s="2" t="s">
         <v>66</v>
@@ -18307,7 +18259,7 @@
         <v>63</v>
       </c>
       <c r="E227" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F227" s="2" t="s">
         <v>66</v>
@@ -18348,7 +18300,7 @@
         <v>63</v>
       </c>
       <c r="E228" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F228" s="2" t="s">
         <v>66</v>
@@ -18389,7 +18341,7 @@
         <v>63</v>
       </c>
       <c r="E229" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F229" s="2" t="s">
         <v>66</v>
@@ -18430,7 +18382,7 @@
         <v>63</v>
       </c>
       <c r="E230" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F230" s="2" t="s">
         <v>66</v>
@@ -18471,7 +18423,7 @@
         <v>63</v>
       </c>
       <c r="E231" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F231" s="2" t="s">
         <v>66</v>
@@ -18512,7 +18464,7 @@
         <v>63</v>
       </c>
       <c r="E232" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F232" s="2" t="s">
         <v>66</v>
@@ -18553,7 +18505,7 @@
         <v>63</v>
       </c>
       <c r="E233" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F233" s="2" t="s">
         <v>66</v>
@@ -18594,7 +18546,7 @@
         <v>63</v>
       </c>
       <c r="E234" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F234" s="2" t="s">
         <v>66</v>
@@ -18635,7 +18587,7 @@
         <v>27</v>
       </c>
       <c r="E235" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F235" s="2" t="s">
         <v>66</v>
@@ -18676,7 +18628,7 @@
         <v>122</v>
       </c>
       <c r="E236" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F236" s="7" t="s">
         <v>66</v>
@@ -18717,7 +18669,7 @@
         <v>122</v>
       </c>
       <c r="E237" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F237" s="7" t="s">
         <v>66</v>
@@ -18758,7 +18710,7 @@
         <v>122</v>
       </c>
       <c r="E238" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F238" s="7" t="s">
         <v>66</v>
@@ -18799,7 +18751,7 @@
         <v>122</v>
       </c>
       <c r="E239" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F239" s="7" t="s">
         <v>66</v>
@@ -18840,7 +18792,7 @@
         <v>122</v>
       </c>
       <c r="E240" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F240" s="7" t="s">
         <v>66</v>
@@ -18881,7 +18833,7 @@
         <v>122</v>
       </c>
       <c r="E241" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F241" s="7" t="s">
         <v>66</v>
@@ -18922,7 +18874,7 @@
         <v>121</v>
       </c>
       <c r="E242" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F242" s="7" t="s">
         <v>66</v>
@@ -18963,7 +18915,7 @@
         <v>121</v>
       </c>
       <c r="E243" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F243" s="7" t="s">
         <v>66</v>
@@ -19004,7 +18956,7 @@
         <v>121</v>
       </c>
       <c r="E244" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F244" s="7" t="s">
         <v>66</v>
@@ -19045,7 +18997,7 @@
         <v>121</v>
       </c>
       <c r="E245" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F245" s="7" t="s">
         <v>66</v>
@@ -19086,7 +19038,7 @@
         <v>121</v>
       </c>
       <c r="E246" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F246" s="7" t="s">
         <v>66</v>
@@ -19127,7 +19079,7 @@
         <v>121</v>
       </c>
       <c r="E247" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F247" s="7" t="s">
         <v>66</v>
@@ -19168,7 +19120,7 @@
         <v>121</v>
       </c>
       <c r="E248" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F248" s="7" t="s">
         <v>66</v>
@@ -19209,7 +19161,7 @@
         <v>121</v>
       </c>
       <c r="E249" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F249" s="7" t="s">
         <v>66</v>
@@ -19250,7 +19202,7 @@
         <v>121</v>
       </c>
       <c r="E250" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F250" s="7" t="s">
         <v>66</v>
@@ -19291,7 +19243,7 @@
         <v>121</v>
       </c>
       <c r="E251" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F251" s="7" t="s">
         <v>66</v>
@@ -19332,7 +19284,7 @@
         <v>121</v>
       </c>
       <c r="E252" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F252" s="7" t="s">
         <v>66</v>
@@ -19373,7 +19325,7 @@
         <v>121</v>
       </c>
       <c r="E253" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F253" s="7" t="s">
         <v>66</v>
@@ -19414,7 +19366,7 @@
         <v>123</v>
       </c>
       <c r="E254" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F254" s="7" t="s">
         <v>66</v>
@@ -19455,7 +19407,7 @@
         <v>124</v>
       </c>
       <c r="E255" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F255" s="7" t="s">
         <v>66</v>
@@ -19496,7 +19448,7 @@
         <v>124</v>
       </c>
       <c r="E256" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F256" s="7" t="s">
         <v>66</v>
@@ -19537,7 +19489,7 @@
         <v>124</v>
       </c>
       <c r="E257" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F257" s="7" t="s">
         <v>66</v>
@@ -19578,7 +19530,7 @@
         <v>124</v>
       </c>
       <c r="E258" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F258" s="7" t="s">
         <v>66</v>
@@ -19619,7 +19571,7 @@
         <v>124</v>
       </c>
       <c r="E259" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F259" s="7" t="s">
         <v>66</v>
@@ -19660,7 +19612,7 @@
         <v>124</v>
       </c>
       <c r="E260" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F260" s="7" t="s">
         <v>66</v>
@@ -19701,7 +19653,7 @@
         <v>124</v>
       </c>
       <c r="E261" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F261" s="7" t="s">
         <v>66</v>
@@ -19742,7 +19694,7 @@
         <v>124</v>
       </c>
       <c r="E262" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F262" s="7" t="s">
         <v>66</v>
@@ -19783,7 +19735,7 @@
         <v>124</v>
       </c>
       <c r="E263" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F263" s="7" t="s">
         <v>66</v>
@@ -19824,7 +19776,7 @@
         <v>124</v>
       </c>
       <c r="E264" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F264" s="7" t="s">
         <v>66</v>
@@ -19865,7 +19817,7 @@
         <v>124</v>
       </c>
       <c r="E265" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F265" s="7" t="s">
         <v>66</v>
@@ -19906,7 +19858,7 @@
         <v>124</v>
       </c>
       <c r="E266" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F266" s="7" t="s">
         <v>66</v>
@@ -19947,7 +19899,7 @@
         <v>124</v>
       </c>
       <c r="E267" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F267" s="7" t="s">
         <v>66</v>
@@ -19988,7 +19940,7 @@
         <v>124</v>
       </c>
       <c r="E268" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F268" s="7" t="s">
         <v>66</v>
@@ -20029,7 +19981,7 @@
         <v>142</v>
       </c>
       <c r="E269" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F269" s="7" t="s">
         <v>66</v>
@@ -20070,7 +20022,7 @@
         <v>142</v>
       </c>
       <c r="E270" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F270" s="7" t="s">
         <v>66</v>
@@ -20111,7 +20063,7 @@
         <v>145</v>
       </c>
       <c r="E271" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F271" s="7" t="s">
         <v>66</v>
@@ -20152,7 +20104,7 @@
         <v>145</v>
       </c>
       <c r="E272" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F272" s="7" t="s">
         <v>66</v>
@@ -20193,7 +20145,7 @@
         <v>145</v>
       </c>
       <c r="E273" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F273" s="7" t="s">
         <v>66</v>
@@ -20234,7 +20186,7 @@
         <v>145</v>
       </c>
       <c r="E274" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F274" s="7" t="s">
         <v>66</v>
@@ -20275,7 +20227,7 @@
         <v>145</v>
       </c>
       <c r="E275" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F275" s="7" t="s">
         <v>66</v>
@@ -20316,7 +20268,7 @@
         <v>145</v>
       </c>
       <c r="E276" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F276" s="7" t="s">
         <v>66</v>
@@ -20357,7 +20309,7 @@
         <v>145</v>
       </c>
       <c r="E277" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F277" s="7" t="s">
         <v>66</v>
@@ -20398,7 +20350,7 @@
         <v>145</v>
       </c>
       <c r="E278" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F278" s="7" t="s">
         <v>66</v>
@@ -20439,7 +20391,7 @@
         <v>145</v>
       </c>
       <c r="E279" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F279" s="7" t="s">
         <v>66</v>
@@ -20480,7 +20432,7 @@
         <v>145</v>
       </c>
       <c r="E280" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F280" s="7" t="s">
         <v>66</v>
@@ -20521,7 +20473,7 @@
         <v>145</v>
       </c>
       <c r="E281" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F281" s="7" t="s">
         <v>66</v>
@@ -20562,7 +20514,7 @@
         <v>145</v>
       </c>
       <c r="E282" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F282" s="7" t="s">
         <v>66</v>
@@ -20603,7 +20555,7 @@
         <v>145</v>
       </c>
       <c r="E283" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F283" s="7" t="s">
         <v>66</v>
@@ -20644,7 +20596,7 @@
         <v>145</v>
       </c>
       <c r="E284" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F284" s="7" t="s">
         <v>66</v>
@@ -20685,7 +20637,7 @@
         <v>141</v>
       </c>
       <c r="E285" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F285" s="7" t="s">
         <v>66</v>
@@ -20726,7 +20678,7 @@
         <v>141</v>
       </c>
       <c r="E286" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F286" s="7" t="s">
         <v>66</v>
@@ -20767,7 +20719,7 @@
         <v>143</v>
       </c>
       <c r="E287" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F287" s="7" t="s">
         <v>66</v>
@@ -20808,7 +20760,7 @@
         <v>143</v>
       </c>
       <c r="E288" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F288" s="7" t="s">
         <v>66</v>
@@ -20849,7 +20801,7 @@
         <v>143</v>
       </c>
       <c r="E289" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F289" s="7" t="s">
         <v>66</v>
@@ -20890,7 +20842,7 @@
         <v>143</v>
       </c>
       <c r="E290" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F290" s="7" t="s">
         <v>66</v>
@@ -20931,7 +20883,7 @@
         <v>143</v>
       </c>
       <c r="E291" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F291" s="7" t="s">
         <v>66</v>
@@ -20972,7 +20924,7 @@
         <v>143</v>
       </c>
       <c r="E292" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F292" s="7" t="s">
         <v>66</v>
@@ -21013,7 +20965,7 @@
         <v>144</v>
       </c>
       <c r="E293" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F293" s="7" t="s">
         <v>66</v>
@@ -21054,7 +21006,7 @@
         <v>144</v>
       </c>
       <c r="E294" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F294" s="7" t="s">
         <v>66</v>
@@ -21095,7 +21047,7 @@
         <v>144</v>
       </c>
       <c r="E295" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F295" s="7" t="s">
         <v>66</v>
@@ -21136,7 +21088,7 @@
         <v>144</v>
       </c>
       <c r="E296" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F296" s="7" t="s">
         <v>66</v>
@@ -21177,7 +21129,7 @@
         <v>144</v>
       </c>
       <c r="E297" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F297" s="7" t="s">
         <v>66</v>
@@ -21218,7 +21170,7 @@
         <v>144</v>
       </c>
       <c r="E298" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F298" s="7" t="s">
         <v>66</v>
@@ -21259,7 +21211,7 @@
         <v>140</v>
       </c>
       <c r="E299" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F299" s="7" t="s">
         <v>66</v>
@@ -21300,7 +21252,7 @@
         <v>140</v>
       </c>
       <c r="E300" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F300" s="7" t="s">
         <v>66</v>
@@ -21341,7 +21293,7 @@
         <v>140</v>
       </c>
       <c r="E301" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F301" s="7" t="s">
         <v>66</v>
@@ -21382,7 +21334,7 @@
         <v>140</v>
       </c>
       <c r="E302" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F302" s="7" t="s">
         <v>66</v>
@@ -21423,7 +21375,7 @@
         <v>140</v>
       </c>
       <c r="E303" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F303" s="7" t="s">
         <v>66</v>
@@ -21464,7 +21416,7 @@
         <v>140</v>
       </c>
       <c r="E304" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F304" s="7" t="s">
         <v>66</v>
@@ -21505,7 +21457,7 @@
         <v>140</v>
       </c>
       <c r="E305" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="F305" s="7" t="s">
         <v>66</v>
@@ -21546,7 +21498,7 @@
         <v>131</v>
       </c>
       <c r="E306" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F306" s="7" t="s">
         <v>66</v>
@@ -21587,7 +21539,7 @@
         <v>131</v>
       </c>
       <c r="E307" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F307" s="7" t="s">
         <v>66</v>
@@ -21628,7 +21580,7 @@
         <v>131</v>
       </c>
       <c r="E308" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F308" s="7" t="s">
         <v>66</v>
@@ -21669,7 +21621,7 @@
         <v>131</v>
       </c>
       <c r="E309" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F309" s="7" t="s">
         <v>66</v>
@@ -21710,7 +21662,7 @@
         <v>131</v>
       </c>
       <c r="E310" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F310" s="7" t="s">
         <v>66</v>
@@ -21751,7 +21703,7 @@
         <v>131</v>
       </c>
       <c r="E311" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F311" s="7" t="s">
         <v>66</v>
@@ -21792,7 +21744,7 @@
         <v>131</v>
       </c>
       <c r="E312" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F312" s="7" t="s">
         <v>66</v>
@@ -21833,7 +21785,7 @@
         <v>131</v>
       </c>
       <c r="E313" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F313" s="7" t="s">
         <v>66</v>
@@ -21874,7 +21826,7 @@
         <v>131</v>
       </c>
       <c r="E314" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F314" s="7" t="s">
         <v>66</v>
@@ -21915,7 +21867,7 @@
         <v>132</v>
       </c>
       <c r="E315" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F315" s="7" t="s">
         <v>66</v>
@@ -21956,7 +21908,7 @@
         <v>132</v>
       </c>
       <c r="E316" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F316" s="7" t="s">
         <v>66</v>
@@ -21997,7 +21949,7 @@
         <v>132</v>
       </c>
       <c r="E317" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F317" s="7" t="s">
         <v>66</v>
@@ -22038,7 +21990,7 @@
         <v>132</v>
       </c>
       <c r="E318" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F318" s="7" t="s">
         <v>66</v>
@@ -22079,7 +22031,7 @@
         <v>132</v>
       </c>
       <c r="E319" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F319" s="7" t="s">
         <v>66</v>
@@ -22120,7 +22072,7 @@
         <v>132</v>
       </c>
       <c r="E320" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F320" s="7" t="s">
         <v>66</v>
@@ -22161,7 +22113,7 @@
         <v>130</v>
       </c>
       <c r="E321" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F321" s="7" t="s">
         <v>66</v>
@@ -22202,7 +22154,7 @@
         <v>130</v>
       </c>
       <c r="E322" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F322" s="7" t="s">
         <v>66</v>
@@ -22243,7 +22195,7 @@
         <v>130</v>
       </c>
       <c r="E323" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F323" s="7" t="s">
         <v>66</v>
@@ -22284,7 +22236,7 @@
         <v>130</v>
       </c>
       <c r="E324" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F324" s="7" t="s">
         <v>66</v>
@@ -22325,7 +22277,7 @@
         <v>130</v>
       </c>
       <c r="E325" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F325" s="7" t="s">
         <v>66</v>
@@ -22366,7 +22318,7 @@
         <v>130</v>
       </c>
       <c r="E326" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F326" s="7" t="s">
         <v>66</v>
@@ -22407,7 +22359,7 @@
         <v>130</v>
       </c>
       <c r="E327" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F327" s="7" t="s">
         <v>66</v>
@@ -22448,7 +22400,7 @@
         <v>130</v>
       </c>
       <c r="E328" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F328" s="7" t="s">
         <v>66</v>
@@ -22489,7 +22441,7 @@
         <v>130</v>
       </c>
       <c r="E329" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F329" s="7" t="s">
         <v>66</v>
@@ -22530,7 +22482,7 @@
         <v>130</v>
       </c>
       <c r="E330" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F330" s="7" t="s">
         <v>66</v>
@@ -22571,7 +22523,7 @@
         <v>130</v>
       </c>
       <c r="E331" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F331" s="7" t="s">
         <v>66</v>
@@ -22612,7 +22564,7 @@
         <v>130</v>
       </c>
       <c r="E332" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F332" s="7" t="s">
         <v>66</v>
@@ -22653,7 +22605,7 @@
         <v>130</v>
       </c>
       <c r="E333" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F333" s="7" t="s">
         <v>66</v>
@@ -22694,7 +22646,7 @@
         <v>130</v>
       </c>
       <c r="E334" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F334" s="7" t="s">
         <v>66</v>
@@ -22735,7 +22687,7 @@
         <v>130</v>
       </c>
       <c r="E335" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F335" s="7" t="s">
         <v>66</v>
@@ -22776,7 +22728,7 @@
         <v>130</v>
       </c>
       <c r="E336" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F336" s="7" t="s">
         <v>66</v>
@@ -22817,7 +22769,7 @@
         <v>130</v>
       </c>
       <c r="E337" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F337" s="7" t="s">
         <v>66</v>
@@ -22858,7 +22810,7 @@
         <v>130</v>
       </c>
       <c r="E338" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F338" s="7" t="s">
         <v>66</v>
@@ -22899,7 +22851,7 @@
         <v>130</v>
       </c>
       <c r="E339" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F339" s="7" t="s">
         <v>66</v>
@@ -22940,7 +22892,7 @@
         <v>130</v>
       </c>
       <c r="E340" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F340" s="7" t="s">
         <v>66</v>
@@ -22981,7 +22933,7 @@
         <v>134</v>
       </c>
       <c r="E341" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F341" s="7" t="s">
         <v>66</v>
@@ -23022,7 +22974,7 @@
         <v>133</v>
       </c>
       <c r="E342" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F342" s="7" t="s">
         <v>66</v>
@@ -23063,7 +23015,7 @@
         <v>133</v>
       </c>
       <c r="E343" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F343" s="7" t="s">
         <v>66</v>
@@ -23104,7 +23056,7 @@
         <v>133</v>
       </c>
       <c r="E344" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F344" s="7" t="s">
         <v>66</v>
@@ -23145,7 +23097,7 @@
         <v>117</v>
       </c>
       <c r="E345" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F345" s="7" t="s">
         <v>66</v>
@@ -23186,7 +23138,7 @@
         <v>117</v>
       </c>
       <c r="E346" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F346" s="7" t="s">
         <v>66</v>
@@ -23227,7 +23179,7 @@
         <v>117</v>
       </c>
       <c r="E347" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F347" s="7" t="s">
         <v>66</v>
@@ -23268,7 +23220,7 @@
         <v>117</v>
       </c>
       <c r="E348" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F348" s="7" t="s">
         <v>66</v>
@@ -23309,7 +23261,7 @@
         <v>117</v>
       </c>
       <c r="E349" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F349" s="7" t="s">
         <v>66</v>
@@ -23350,7 +23302,7 @@
         <v>117</v>
       </c>
       <c r="E350" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F350" s="7" t="s">
         <v>66</v>
@@ -23391,7 +23343,7 @@
         <v>117</v>
       </c>
       <c r="E351" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F351" s="7" t="s">
         <v>66</v>
@@ -23432,7 +23384,7 @@
         <v>117</v>
       </c>
       <c r="E352" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F352" s="7" t="s">
         <v>66</v>
@@ -23473,7 +23425,7 @@
         <v>117</v>
       </c>
       <c r="E353" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F353" s="7" t="s">
         <v>66</v>
@@ -23514,7 +23466,7 @@
         <v>120</v>
       </c>
       <c r="E354" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F354" s="7" t="s">
         <v>66</v>
@@ -23555,7 +23507,7 @@
         <v>120</v>
       </c>
       <c r="E355" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F355" s="7" t="s">
         <v>66</v>
@@ -23596,7 +23548,7 @@
         <v>120</v>
       </c>
       <c r="E356" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F356" s="7" t="s">
         <v>66</v>
@@ -23637,7 +23589,7 @@
         <v>120</v>
       </c>
       <c r="E357" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F357" s="7" t="s">
         <v>66</v>
@@ -23678,7 +23630,7 @@
         <v>120</v>
       </c>
       <c r="E358" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F358" s="7" t="s">
         <v>66</v>
@@ -23719,7 +23671,7 @@
         <v>120</v>
       </c>
       <c r="E359" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F359" s="7" t="s">
         <v>66</v>
@@ -23760,7 +23712,7 @@
         <v>120</v>
       </c>
       <c r="E360" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F360" s="7" t="s">
         <v>66</v>
@@ -23801,7 +23753,7 @@
         <v>120</v>
       </c>
       <c r="E361" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F361" s="7" t="s">
         <v>66</v>
@@ -23842,7 +23794,7 @@
         <v>118</v>
       </c>
       <c r="E362" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F362" s="7" t="s">
         <v>66</v>
@@ -23883,7 +23835,7 @@
         <v>118</v>
       </c>
       <c r="E363" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F363" s="7" t="s">
         <v>66</v>
@@ -23924,7 +23876,7 @@
         <v>118</v>
       </c>
       <c r="E364" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F364" s="7" t="s">
         <v>66</v>
@@ -23965,7 +23917,7 @@
         <v>118</v>
       </c>
       <c r="E365" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F365" s="7" t="s">
         <v>66</v>
@@ -24006,7 +23958,7 @@
         <v>118</v>
       </c>
       <c r="E366" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F366" s="7" t="s">
         <v>66</v>
@@ -24047,7 +23999,7 @@
         <v>118</v>
       </c>
       <c r="E367" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F367" s="7" t="s">
         <v>66</v>
@@ -24088,7 +24040,7 @@
         <v>118</v>
       </c>
       <c r="E368" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F368" s="7" t="s">
         <v>66</v>
@@ -24129,7 +24081,7 @@
         <v>118</v>
       </c>
       <c r="E369" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F369" s="7" t="s">
         <v>66</v>
@@ -24170,7 +24122,7 @@
         <v>118</v>
       </c>
       <c r="E370" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F370" s="7" t="s">
         <v>66</v>
@@ -24211,7 +24163,7 @@
         <v>118</v>
       </c>
       <c r="E371" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F371" s="7" t="s">
         <v>66</v>
@@ -24252,7 +24204,7 @@
         <v>118</v>
       </c>
       <c r="E372" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F372" s="7" t="s">
         <v>66</v>
@@ -24293,7 +24245,7 @@
         <v>118</v>
       </c>
       <c r="E373" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F373" s="7" t="s">
         <v>66</v>
@@ -24334,7 +24286,7 @@
         <v>118</v>
       </c>
       <c r="E374" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F374" s="7" t="s">
         <v>66</v>
@@ -24375,7 +24327,7 @@
         <v>118</v>
       </c>
       <c r="E375" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F375" s="7" t="s">
         <v>66</v>
@@ -24416,7 +24368,7 @@
         <v>119</v>
       </c>
       <c r="E376" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F376" s="7" t="s">
         <v>66</v>
@@ -24457,7 +24409,7 @@
         <v>119</v>
       </c>
       <c r="E377" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F377" s="7" t="s">
         <v>66</v>
@@ -24498,7 +24450,7 @@
         <v>119</v>
       </c>
       <c r="E378" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F378" s="7" t="s">
         <v>66</v>
@@ -24539,7 +24491,7 @@
         <v>119</v>
       </c>
       <c r="E379" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F379" s="7" t="s">
         <v>66</v>
@@ -24580,7 +24532,7 @@
         <v>119</v>
       </c>
       <c r="E380" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F380" s="7" t="s">
         <v>66</v>
@@ -24621,7 +24573,7 @@
         <v>119</v>
       </c>
       <c r="E381" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F381" s="7" t="s">
         <v>66</v>
@@ -24662,7 +24614,7 @@
         <v>119</v>
       </c>
       <c r="E382" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F382" s="7" t="s">
         <v>66</v>
@@ -24703,7 +24655,7 @@
         <v>119</v>
       </c>
       <c r="E383" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F383" s="7" t="s">
         <v>66</v>
@@ -24744,7 +24696,7 @@
         <v>119</v>
       </c>
       <c r="E384" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F384" s="7" t="s">
         <v>66</v>
@@ -24785,7 +24737,7 @@
         <v>137</v>
       </c>
       <c r="E385" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F385" s="7" t="s">
         <v>66</v>
@@ -24826,7 +24778,7 @@
         <v>139</v>
       </c>
       <c r="E386" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F386" s="7" t="s">
         <v>66</v>
@@ -24867,7 +24819,7 @@
         <v>139</v>
       </c>
       <c r="E387" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F387" s="7" t="s">
         <v>66</v>
@@ -24908,7 +24860,7 @@
         <v>139</v>
       </c>
       <c r="E388" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F388" s="7" t="s">
         <v>66</v>
@@ -24949,7 +24901,7 @@
         <v>139</v>
       </c>
       <c r="E389" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F389" s="7" t="s">
         <v>66</v>
@@ -24990,7 +24942,7 @@
         <v>139</v>
       </c>
       <c r="E390" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F390" s="7" t="s">
         <v>66</v>
@@ -25031,7 +24983,7 @@
         <v>139</v>
       </c>
       <c r="E391" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F391" s="7" t="s">
         <v>66</v>
@@ -25072,7 +25024,7 @@
         <v>139</v>
       </c>
       <c r="E392" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F392" s="7" t="s">
         <v>66</v>
@@ -25113,7 +25065,7 @@
         <v>139</v>
       </c>
       <c r="E393" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F393" s="7" t="s">
         <v>66</v>
@@ -25154,7 +25106,7 @@
         <v>139</v>
       </c>
       <c r="E394" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F394" s="7" t="s">
         <v>66</v>
@@ -25195,7 +25147,7 @@
         <v>139</v>
       </c>
       <c r="E395" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F395" s="7" t="s">
         <v>66</v>
@@ -25236,7 +25188,7 @@
         <v>139</v>
       </c>
       <c r="E396" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F396" s="7" t="s">
         <v>66</v>
@@ -25277,7 +25229,7 @@
         <v>139</v>
       </c>
       <c r="E397" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F397" s="7" t="s">
         <v>66</v>
@@ -25318,7 +25270,7 @@
         <v>139</v>
       </c>
       <c r="E398" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F398" s="7" t="s">
         <v>66</v>
@@ -25359,7 +25311,7 @@
         <v>139</v>
       </c>
       <c r="E399" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F399" s="7" t="s">
         <v>66</v>
@@ -25400,7 +25352,7 @@
         <v>139</v>
       </c>
       <c r="E400" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F400" s="7" t="s">
         <v>66</v>
@@ -25441,7 +25393,7 @@
         <v>139</v>
       </c>
       <c r="E401" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F401" s="7" t="s">
         <v>66</v>
@@ -25482,7 +25434,7 @@
         <v>139</v>
       </c>
       <c r="E402" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F402" s="7" t="s">
         <v>66</v>
@@ -25523,7 +25475,7 @@
         <v>139</v>
       </c>
       <c r="E403" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F403" s="7" t="s">
         <v>66</v>
@@ -25564,7 +25516,7 @@
         <v>139</v>
       </c>
       <c r="E404" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F404" s="7" t="s">
         <v>66</v>
@@ -25605,7 +25557,7 @@
         <v>136</v>
       </c>
       <c r="E405" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F405" s="7" t="s">
         <v>66</v>
@@ -25646,7 +25598,7 @@
         <v>136</v>
       </c>
       <c r="E406" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F406" s="7" t="s">
         <v>66</v>
@@ -25687,7 +25639,7 @@
         <v>136</v>
       </c>
       <c r="E407" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F407" s="7" t="s">
         <v>66</v>
@@ -25728,7 +25680,7 @@
         <v>136</v>
       </c>
       <c r="E408" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F408" s="7" t="s">
         <v>66</v>
@@ -25769,7 +25721,7 @@
         <v>136</v>
       </c>
       <c r="E409" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F409" s="7" t="s">
         <v>66</v>
@@ -25810,7 +25762,7 @@
         <v>136</v>
       </c>
       <c r="E410" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F410" s="7" t="s">
         <v>66</v>
@@ -25851,7 +25803,7 @@
         <v>136</v>
       </c>
       <c r="E411" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F411" s="7" t="s">
         <v>66</v>
@@ -25892,7 +25844,7 @@
         <v>136</v>
       </c>
       <c r="E412" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F412" s="7" t="s">
         <v>66</v>
@@ -25933,7 +25885,7 @@
         <v>136</v>
       </c>
       <c r="E413" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F413" s="7" t="s">
         <v>66</v>
@@ -25974,7 +25926,7 @@
         <v>136</v>
       </c>
       <c r="E414" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F414" s="7" t="s">
         <v>66</v>
@@ -26015,7 +25967,7 @@
         <v>135</v>
       </c>
       <c r="E415" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F415" s="7" t="s">
         <v>66</v>
@@ -26056,7 +26008,7 @@
         <v>135</v>
       </c>
       <c r="E416" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F416" s="7" t="s">
         <v>66</v>
@@ -26097,7 +26049,7 @@
         <v>135</v>
       </c>
       <c r="E417" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F417" s="7" t="s">
         <v>66</v>
@@ -26138,7 +26090,7 @@
         <v>135</v>
       </c>
       <c r="E418" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F418" s="7" t="s">
         <v>66</v>
@@ -26179,7 +26131,7 @@
         <v>135</v>
       </c>
       <c r="E419" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F419" s="7" t="s">
         <v>66</v>
@@ -26220,7 +26172,7 @@
         <v>138</v>
       </c>
       <c r="E420" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F420" s="7" t="s">
         <v>66</v>
@@ -26261,7 +26213,7 @@
         <v>138</v>
       </c>
       <c r="E421" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F421" s="7" t="s">
         <v>66</v>
@@ -26302,7 +26254,7 @@
         <v>138</v>
       </c>
       <c r="E422" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F422" s="7" t="s">
         <v>66</v>
@@ -26343,7 +26295,7 @@
         <v>138</v>
       </c>
       <c r="E423" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F423" s="7" t="s">
         <v>66</v>
@@ -26384,7 +26336,7 @@
         <v>138</v>
       </c>
       <c r="E424" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F424" s="7" t="s">
         <v>66</v>
@@ -26425,7 +26377,7 @@
         <v>125</v>
       </c>
       <c r="E425" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F425" s="7" t="s">
         <v>66</v>
@@ -26466,7 +26418,7 @@
         <v>125</v>
       </c>
       <c r="E426" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F426" s="7" t="s">
         <v>66</v>
@@ -26507,7 +26459,7 @@
         <v>125</v>
       </c>
       <c r="E427" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F427" s="7" t="s">
         <v>66</v>
@@ -26548,7 +26500,7 @@
         <v>125</v>
       </c>
       <c r="E428" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F428" s="7" t="s">
         <v>66</v>
@@ -26589,7 +26541,7 @@
         <v>125</v>
       </c>
       <c r="E429" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F429" s="7" t="s">
         <v>66</v>
@@ -26630,7 +26582,7 @@
         <v>125</v>
       </c>
       <c r="E430" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F430" s="7" t="s">
         <v>66</v>
@@ -26671,7 +26623,7 @@
         <v>125</v>
       </c>
       <c r="E431" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F431" s="7" t="s">
         <v>66</v>
@@ -26712,7 +26664,7 @@
         <v>125</v>
       </c>
       <c r="E432" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F432" s="7" t="s">
         <v>66</v>
@@ -26753,7 +26705,7 @@
         <v>125</v>
       </c>
       <c r="E433" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F433" s="7" t="s">
         <v>66</v>
@@ -26794,7 +26746,7 @@
         <v>125</v>
       </c>
       <c r="E434" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F434" s="7" t="s">
         <v>66</v>
@@ -26835,7 +26787,7 @@
         <v>128</v>
       </c>
       <c r="E435" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F435" s="7" t="s">
         <v>66</v>
@@ -26876,7 +26828,7 @@
         <v>128</v>
       </c>
       <c r="E436" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F436" s="7" t="s">
         <v>66</v>
@@ -26917,7 +26869,7 @@
         <v>128</v>
       </c>
       <c r="E437" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F437" s="7" t="s">
         <v>66</v>
@@ -26958,7 +26910,7 @@
         <v>128</v>
       </c>
       <c r="E438" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F438" s="7" t="s">
         <v>66</v>
@@ -26999,7 +26951,7 @@
         <v>128</v>
       </c>
       <c r="E439" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F439" s="7" t="s">
         <v>66</v>
@@ -27040,7 +26992,7 @@
         <v>128</v>
       </c>
       <c r="E440" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F440" s="7" t="s">
         <v>66</v>
@@ -27081,7 +27033,7 @@
         <v>128</v>
       </c>
       <c r="E441" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F441" s="7" t="s">
         <v>66</v>
@@ -27122,7 +27074,7 @@
         <v>128</v>
       </c>
       <c r="E442" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F442" s="7" t="s">
         <v>66</v>
@@ -27163,7 +27115,7 @@
         <v>128</v>
       </c>
       <c r="E443" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F443" s="7" t="s">
         <v>66</v>
@@ -27204,7 +27156,7 @@
         <v>128</v>
       </c>
       <c r="E444" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F444" s="7" t="s">
         <v>66</v>
@@ -27245,7 +27197,7 @@
         <v>128</v>
       </c>
       <c r="E445" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F445" s="7" t="s">
         <v>66</v>
@@ -27286,7 +27238,7 @@
         <v>128</v>
       </c>
       <c r="E446" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F446" s="7" t="s">
         <v>66</v>
@@ -27327,7 +27279,7 @@
         <v>127</v>
       </c>
       <c r="E447" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F447" s="7" t="s">
         <v>66</v>
@@ -27368,7 +27320,7 @@
         <v>127</v>
       </c>
       <c r="E448" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F448" s="7" t="s">
         <v>66</v>
@@ -27409,7 +27361,7 @@
         <v>127</v>
       </c>
       <c r="E449" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F449" s="7" t="s">
         <v>66</v>
@@ -27450,7 +27402,7 @@
         <v>126</v>
       </c>
       <c r="E450" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F450" s="7" t="s">
         <v>66</v>
@@ -27491,7 +27443,7 @@
         <v>126</v>
       </c>
       <c r="E451" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F451" s="7" t="s">
         <v>66</v>
@@ -27532,7 +27484,7 @@
         <v>126</v>
       </c>
       <c r="E452" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F452" s="7" t="s">
         <v>66</v>
@@ -27573,7 +27525,7 @@
         <v>126</v>
       </c>
       <c r="E453" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F453" s="7" t="s">
         <v>66</v>
@@ -27614,7 +27566,7 @@
         <v>126</v>
       </c>
       <c r="E454" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F454" s="7" t="s">
         <v>66</v>
@@ -27655,7 +27607,7 @@
         <v>129</v>
       </c>
       <c r="E455" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F455" s="7" t="s">
         <v>66</v>
@@ -27696,7 +27648,7 @@
         <v>129</v>
       </c>
       <c r="E456" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F456" s="7" t="s">
         <v>66</v>
@@ -27737,7 +27689,7 @@
         <v>129</v>
       </c>
       <c r="E457" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F457" s="7" t="s">
         <v>66</v>
@@ -27778,7 +27730,7 @@
         <v>129</v>
       </c>
       <c r="E458" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F458" s="7" t="s">
         <v>66</v>
@@ -27819,7 +27771,7 @@
         <v>129</v>
       </c>
       <c r="E459" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F459" s="7" t="s">
         <v>66</v>
@@ -27860,7 +27812,7 @@
         <v>129</v>
       </c>
       <c r="E460" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F460" s="7" t="s">
         <v>66</v>
@@ -27901,7 +27853,7 @@
         <v>129</v>
       </c>
       <c r="E461" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F461" s="7" t="s">
         <v>66</v>
@@ -27942,7 +27894,7 @@
         <v>129</v>
       </c>
       <c r="E462" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F462" s="7" t="s">
         <v>66</v>
@@ -27983,7 +27935,7 @@
         <v>129</v>
       </c>
       <c r="E463" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F463" s="7" t="s">
         <v>66</v>
@@ -28024,7 +27976,7 @@
         <v>129</v>
       </c>
       <c r="E464" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F464" s="7" t="s">
         <v>66</v>
@@ -28065,7 +28017,7 @@
         <v>115</v>
       </c>
       <c r="E465" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F465" s="7" t="s">
         <v>24</v>
@@ -28106,7 +28058,7 @@
         <v>116</v>
       </c>
       <c r="E466" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F466" s="7" t="s">
         <v>24</v>
@@ -28147,7 +28099,7 @@
         <v>116</v>
       </c>
       <c r="E467" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F467" s="7" t="s">
         <v>24</v>
@@ -28188,7 +28140,7 @@
         <v>116</v>
       </c>
       <c r="E468" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F468" s="7" t="s">
         <v>24</v>
@@ -28229,7 +28181,7 @@
         <v>112</v>
       </c>
       <c r="E469" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F469" s="7" t="s">
         <v>24</v>
@@ -28270,7 +28222,7 @@
         <v>112</v>
       </c>
       <c r="E470" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F470" s="7" t="s">
         <v>24</v>
@@ -28311,7 +28263,7 @@
         <v>113</v>
       </c>
       <c r="E471" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F471" s="7" t="s">
         <v>24</v>
@@ -28352,7 +28304,7 @@
         <v>113</v>
       </c>
       <c r="E472" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F472" s="7" t="s">
         <v>24</v>
@@ -28393,7 +28345,7 @@
         <v>108</v>
       </c>
       <c r="E473" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F473" s="7" t="s">
         <v>24</v>
@@ -28434,7 +28386,7 @@
         <v>108</v>
       </c>
       <c r="E474" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F474" s="7" t="s">
         <v>24</v>
@@ -28475,7 +28427,7 @@
         <v>109</v>
       </c>
       <c r="E475" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F475" s="7" t="s">
         <v>24</v>
@@ -28516,7 +28468,7 @@
         <v>109</v>
       </c>
       <c r="E476" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F476" s="7" t="s">
         <v>24</v>
@@ -28557,7 +28509,7 @@
         <v>110</v>
       </c>
       <c r="E477" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F477" s="7" t="s">
         <v>24</v>
@@ -28598,7 +28550,7 @@
         <v>110</v>
       </c>
       <c r="E478" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F478" s="7" t="s">
         <v>24</v>
@@ -28639,7 +28591,7 @@
         <v>110</v>
       </c>
       <c r="E479" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F479" s="7" t="s">
         <v>24</v>
@@ -28680,7 +28632,7 @@
         <v>110</v>
       </c>
       <c r="E480" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F480" s="7" t="s">
         <v>24</v>
@@ -28721,7 +28673,7 @@
         <v>2</v>
       </c>
       <c r="E481" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F481" s="2" t="s">
         <v>4</v>
@@ -28762,7 +28714,7 @@
         <v>2</v>
       </c>
       <c r="E482" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F482" s="2" t="s">
         <v>4</v>
@@ -28803,7 +28755,7 @@
         <v>2</v>
       </c>
       <c r="E483" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F483" s="2" t="s">
         <v>4</v>
@@ -28844,7 +28796,7 @@
         <v>2</v>
       </c>
       <c r="E484" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F484" s="2" t="s">
         <v>4</v>
@@ -28885,7 +28837,7 @@
         <v>2</v>
       </c>
       <c r="E485" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F485" s="2" t="s">
         <v>4</v>
@@ -28926,7 +28878,7 @@
         <v>2</v>
       </c>
       <c r="E486" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F486" s="2" t="s">
         <v>4</v>
@@ -28967,7 +28919,7 @@
         <v>2</v>
       </c>
       <c r="E487" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F487" s="2" t="s">
         <v>4</v>
@@ -29008,7 +28960,7 @@
         <v>2</v>
       </c>
       <c r="E488" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="F488" s="2" t="s">
         <v>4</v>

</xml_diff>